<commit_message>
Some restructuring and debugging
NEW 2D ARRAY INSIDE AN ARRAY!!!
</commit_message>
<xml_diff>
--- a/Копия 1.xlsx
+++ b/Копия 1.xlsx
@@ -650,8 +650,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -830,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -886,32 +886,37 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1217,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD67"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
@@ -9398,8 +9403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9408,11 +9413,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="str">
-        <f>Лист1!F23</f>
-        <v>ПТИ</v>
-      </c>
-      <c r="B1" s="36"/>
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
       <c r="E1" s="32"/>
@@ -9424,116 +9426,135 @@
       <c r="K1" s="32"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
-        <f>Лист1!I23</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="16">
-        <v>0</v>
-      </c>
+      <c r="A2" s="31"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="28"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="37">
-        <f>Лист1!H23</f>
-        <v>1.4285714285714285E-2</v>
-      </c>
-      <c r="B3" s="37">
-        <f>B2+A3</f>
-        <v>1.4285714285714285E-2</v>
-      </c>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="37">
-        <f>Лист1!K23</f>
-        <v>1.4285714285714285E-2</v>
-      </c>
-      <c r="B4" s="37">
-        <f t="shared" ref="B4:B11" si="0">B3+A4</f>
-        <v>2.8571428571428571E-2</v>
-      </c>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="28"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
-        <f>Лист1!P23</f>
-        <v>1.4285714285714285E-2</v>
-      </c>
-      <c r="B5" s="37">
-        <f t="shared" si="0"/>
-        <v>4.2857142857142858E-2</v>
-      </c>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="28"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
-        <f>Лист1!J23</f>
-        <v>4.2857142857142858E-2</v>
-      </c>
-      <c r="B6" s="37">
-        <f t="shared" si="0"/>
-        <v>8.5714285714285715E-2</v>
-      </c>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
-        <f>Лист1!O23</f>
-        <v>5.7142857142857141E-2</v>
-      </c>
-      <c r="B7" s="37">
-        <f t="shared" si="0"/>
-        <v>0.14285714285714285</v>
-      </c>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
-        <f>Лист1!N23</f>
-        <v>0.1</v>
-      </c>
-      <c r="B8" s="37">
-        <f t="shared" si="0"/>
-        <v>0.24285714285714285</v>
-      </c>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="28"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
-        <f>Лист1!L23</f>
-        <v>0.15714285714285714</v>
-      </c>
-      <c r="B9" s="37">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+      <c r="A10" s="42" t="str">
+        <f>Лист1!F23</f>
+        <v>ПТИ</v>
+      </c>
+      <c r="B10" s="34">
+        <f>Лист1!I23</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="34">
+        <f>Лист1!H23</f>
+        <v>1.4285714285714285E-2</v>
+      </c>
+      <c r="D10" s="34">
+        <f>Лист1!K23</f>
+        <v>1.4285714285714285E-2</v>
+      </c>
+      <c r="E10" s="34">
+        <f>Лист1!P23</f>
+        <v>1.4285714285714285E-2</v>
+      </c>
+      <c r="F10" s="34">
+        <f>Лист1!J23</f>
+        <v>4.2857142857142858E-2</v>
+      </c>
+      <c r="G10" s="34">
+        <f>Лист1!O23</f>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="H10" s="34">
+        <f>Лист1!N23</f>
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="34">
+        <f>Лист1!L23</f>
+        <v>0.15714285714285714</v>
+      </c>
+      <c r="J10" s="34">
         <f>Лист1!M23</f>
         <v>0.18571428571428572</v>
       </c>
-      <c r="B10" s="37">
+      <c r="K10" s="34">
+        <f>Лист1!G23</f>
+        <v>0.41428571428571431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
+      <c r="B11" s="34">
+        <v>0</v>
+      </c>
+      <c r="C11" s="36">
+        <f>B11+C10</f>
+        <v>1.4285714285714285E-2</v>
+      </c>
+      <c r="D11" s="36">
+        <f t="shared" ref="D11:K11" si="0">C11+D10</f>
+        <v>2.8571428571428571E-2</v>
+      </c>
+      <c r="E11" s="36">
+        <f t="shared" si="0"/>
+        <v>4.2857142857142858E-2</v>
+      </c>
+      <c r="F11" s="36">
+        <f t="shared" si="0"/>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="H11" s="36">
+        <f t="shared" si="0"/>
+        <v>0.24285714285714285</v>
+      </c>
+      <c r="I11" s="36">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="J11" s="36">
         <f t="shared" si="0"/>
         <v>0.58571428571428574</v>
       </c>
-      <c r="C10" s="28"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="37">
-        <f>Лист1!G23</f>
-        <v>0.41428571428571431</v>
-      </c>
-      <c r="B11" s="37">
+      <c r="K11" s="36">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C11" s="28"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="str">
+      <c r="A13" s="37" t="str">
         <f>Лист1!F27</f>
         <v>К,Na</v>
       </c>
@@ -9579,7 +9600,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="35">
         <v>0</v>
       </c>
@@ -9633,53 +9654,53 @@
       <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="str">
+      <c r="A16" s="39" t="str">
         <f>Лист1!F31</f>
         <v>СРБ,АСО</v>
       </c>
-      <c r="B16" s="40">
+      <c r="B16" s="36">
         <f>Лист1!O31</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="36">
         <f>Лист1!P31</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="36">
         <f>Лист1!M31</f>
         <v>4.2857142857142858E-2</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="36">
         <f>Лист1!H31</f>
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="36">
         <f>Лист1!N31</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="36">
         <f>Лист1!L31</f>
         <v>0.11428571428571428</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16" s="36">
         <f>Лист1!J31</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="36">
         <f>Лист1!I31</f>
         <v>0.15714285714285714</v>
       </c>
-      <c r="J16" s="40">
+      <c r="J16" s="36">
         <f>Лист1!G31</f>
         <v>0.18571428571428572</v>
       </c>
-      <c r="K16" s="40">
+      <c r="K16" s="36">
         <f>Лист1!K31</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="35">
         <f>B14+B16</f>
         <v>1.4285714285714285E-2</v>
@@ -9734,53 +9755,53 @@
       <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="str">
+      <c r="A19" s="39" t="str">
         <f>Лист1!F35</f>
         <v>Глюкоза</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="36">
         <f>Лист1!N35</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="36">
         <f>Лист1!O35</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="36">
         <f>Лист1!P35</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="36">
         <f>Лист1!G35</f>
         <v>2.8571428571428571E-2</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="36">
         <f>Лист1!I35</f>
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="36">
         <f>Лист1!M35</f>
         <v>8.5714285714285715E-2</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="36">
         <f>Лист1!H35</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="36">
         <f>Лист1!J35</f>
         <v>0.2</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="36">
         <f>Лист1!L35</f>
         <v>0.2</v>
       </c>
-      <c r="K19" s="40">
+      <c r="K19" s="36">
         <f>Лист1!K35</f>
         <v>0.24285714285714285</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="35">
         <f>B19+B14</f>
         <v>1.4285714285714285E-2</v>
@@ -9835,53 +9856,53 @@
       <c r="J21" s="28"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="str">
+      <c r="A22" s="39" t="str">
         <f>Лист1!F39</f>
         <v>Холестерин</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="36">
         <f>Лист1!O39</f>
         <v>0</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="36">
         <f>Лист1!M39</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="36">
         <f>Лист1!N39</f>
         <v>1.4285714285714285E-2</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="36">
         <f>Лист1!P39</f>
         <v>2.8571428571428571E-2</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="36">
         <f>Лист1!L39</f>
         <v>4.2857142857142858E-2</v>
       </c>
-      <c r="G22" s="40">
+      <c r="G22" s="36">
         <f>Лист1!J39</f>
         <v>0.12857142857142856</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="36">
         <f>Лист1!G39</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="I22" s="40">
+      <c r="I22" s="36">
         <f>Лист1!H39</f>
         <v>0.15714285714285714</v>
       </c>
-      <c r="J22" s="40">
+      <c r="J22" s="36">
         <f>Лист1!K39</f>
         <v>0.2</v>
       </c>
-      <c r="K22" s="40">
+      <c r="K22" s="36">
         <f>Лист1!I39</f>
         <v>0.27142857142857141</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="35">
         <v>0</v>
       </c>
@@ -9926,7 +9947,7 @@
       <c r="A24" s="33"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="str">
+      <c r="A25" s="37" t="str">
         <f>Лист1!F43</f>
         <v>Тимоловая</v>
       </c>
@@ -9972,7 +9993,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="34">
         <f>0+B25</f>
         <v>1.4285714285714285E-2</v>
@@ -10015,7 +10036,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="str">
+      <c r="A28" s="37" t="str">
         <f>Лист1!F47</f>
         <v>Мочев,креат</v>
       </c>
@@ -10061,7 +10082,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
       <c r="D29" s="16"/>
@@ -10074,7 +10095,7 @@
       <c r="K29" s="16"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="str">
+      <c r="A31" s="37" t="str">
         <f>Лист1!F51</f>
         <v>Общ бел</v>
       </c>
@@ -10120,7 +10141,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
       <c r="D32" s="16"/>
@@ -10133,7 +10154,7 @@
       <c r="K32" s="16"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="str">
+      <c r="A34" s="37" t="str">
         <f>Лист1!F55</f>
         <v>Fe,жсс</v>
       </c>
@@ -10179,7 +10200,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
       <c r="D35" s="16"/>
@@ -10192,10 +10213,10 @@
       <c r="K35" s="16"/>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="B34:K34">
-    <sortCondition ref="B34:K34"/>
+  <sortState columnSort="1" ref="B10:K10">
+    <sortCondition ref="B10:K10"/>
   </sortState>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A34:A35"/>
@@ -10205,6 +10226,7 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>